<commit_message>
guess we are done
</commit_message>
<xml_diff>
--- a/lastSundayResult/fulltextresults.xlsx
+++ b/lastSundayResult/fulltextresults.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atz2nd\Dropbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katarzadeh\Dropbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="332">
   <si>
     <t>Query Type</t>
   </si>
@@ -993,6 +993,33 @@
   </si>
   <si>
     <t>504</t>
+  </si>
+  <si>
+    <t>2843136</t>
+  </si>
+  <si>
+    <t>1838399</t>
+  </si>
+  <si>
+    <t>1837520</t>
+  </si>
+  <si>
+    <t>684938</t>
+  </si>
+  <si>
+    <t>627915</t>
+  </si>
+  <si>
+    <t>3473817</t>
+  </si>
+  <si>
+    <t>3614307</t>
+  </si>
+  <si>
+    <t>6045904</t>
+  </si>
+  <si>
+    <t>4180093</t>
   </si>
 </sst>
 </file>
@@ -1020,24 +1047,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="42">
@@ -1585,7 +1600,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1695,27 +1710,45 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1723,30 +1756,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2031,8 +2040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K161"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2082,13 +2091,13 @@
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="51">
+      <c r="A2" s="39">
         <v>1</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="46" t="s">
         <v>17</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -2114,9 +2123,9 @@
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="52"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="41"/>
+      <c r="A3" s="40"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="47"/>
       <c r="D3" s="7" t="s">
         <v>12</v>
       </c>
@@ -2140,9 +2149,9 @@
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="52"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="41"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="47"/>
       <c r="D4" s="7" t="s">
         <v>13</v>
       </c>
@@ -2166,9 +2175,9 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A5" s="52"/>
-      <c r="B5" s="49"/>
-      <c r="C5" s="42"/>
+      <c r="A5" s="40"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="48"/>
       <c r="D5" s="8" t="s">
         <v>14</v>
       </c>
@@ -2192,11 +2201,11 @@
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="52"/>
-      <c r="B6" s="47" t="s">
+      <c r="A6" s="40"/>
+      <c r="B6" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="44" t="s">
+      <c r="C6" s="50" t="s">
         <v>49</v>
       </c>
       <c r="D6" s="6" t="s">
@@ -2222,9 +2231,9 @@
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="52"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="45"/>
+      <c r="A7" s="40"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="51"/>
       <c r="D7" s="7" t="s">
         <v>12</v>
       </c>
@@ -2248,9 +2257,9 @@
       </c>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="52"/>
-      <c r="B8" s="48"/>
-      <c r="C8" s="45"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="51"/>
       <c r="D8" s="7" t="s">
         <v>13</v>
       </c>
@@ -2272,12 +2281,12 @@
       <c r="J8" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="K8" s="39"/>
+      <c r="K8" s="38"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A9" s="52"/>
-      <c r="B9" s="49"/>
-      <c r="C9" s="46"/>
+      <c r="A9" s="40"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="52"/>
       <c r="D9" s="8" t="s">
         <v>14</v>
       </c>
@@ -2301,11 +2310,11 @@
       </c>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="52"/>
-      <c r="B10" s="50" t="s">
+      <c r="A10" s="40"/>
+      <c r="B10" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="45" t="s">
+      <c r="C10" s="51" t="s">
         <v>89</v>
       </c>
       <c r="D10" s="9" t="s">
@@ -2331,9 +2340,9 @@
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="52"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="45"/>
+      <c r="A11" s="40"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="51"/>
       <c r="D11" s="7" t="s">
         <v>12</v>
       </c>
@@ -2357,9 +2366,9 @@
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="52"/>
-      <c r="B12" s="48"/>
-      <c r="C12" s="45"/>
+      <c r="A12" s="40"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="51"/>
       <c r="D12" s="7" t="s">
         <v>13</v>
       </c>
@@ -2383,9 +2392,9 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A13" s="52"/>
-      <c r="B13" s="49"/>
-      <c r="C13" s="46"/>
+      <c r="A13" s="40"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="52"/>
       <c r="D13" s="8" t="s">
         <v>14</v>
       </c>
@@ -2409,11 +2418,11 @@
       </c>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="52"/>
-      <c r="B14" s="50" t="s">
+      <c r="A14" s="40"/>
+      <c r="B14" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="40" t="s">
+      <c r="C14" s="49" t="s">
         <v>310</v>
       </c>
       <c r="D14" s="9" t="s">
@@ -2439,23 +2448,36 @@
       </c>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="52"/>
-      <c r="B15" s="48"/>
-      <c r="C15" s="41"/>
+      <c r="A15" s="40"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="47"/>
       <c r="D15" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="34"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="30"/>
-      <c r="K15" s="37"/>
+      <c r="E15" s="34" t="s">
+        <v>311</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>318</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>314</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>312</v>
+      </c>
+      <c r="I15" s="30" t="s">
+        <v>313</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="K15" s="38"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="52"/>
-      <c r="B16" s="48"/>
-      <c r="C16" s="41"/>
+      <c r="A16" s="40"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="47"/>
       <c r="D16" s="7" t="s">
         <v>13</v>
       </c>
@@ -2477,12 +2499,12 @@
       <c r="J16" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="K16" s="54"/>
+      <c r="K16" s="38"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A17" s="53"/>
-      <c r="B17" s="49"/>
-      <c r="C17" s="42"/>
+      <c r="A17" s="41"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="48"/>
       <c r="D17" s="8" t="s">
         <v>14</v>
       </c>
@@ -2506,13 +2528,13 @@
       </c>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="51">
+      <c r="A18" s="39">
         <v>2</v>
       </c>
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="43" t="s">
+      <c r="C18" s="46" t="s">
         <v>22</v>
       </c>
       <c r="D18" s="6" t="s">
@@ -2538,9 +2560,9 @@
       </c>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="52"/>
-      <c r="B19" s="48"/>
-      <c r="C19" s="41"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="47"/>
       <c r="D19" s="7" t="s">
         <v>12</v>
       </c>
@@ -2564,9 +2586,9 @@
       </c>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="52"/>
-      <c r="B20" s="48"/>
-      <c r="C20" s="41"/>
+      <c r="A20" s="40"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="47"/>
       <c r="D20" s="7" t="s">
         <v>13</v>
       </c>
@@ -2590,9 +2612,9 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A21" s="52"/>
-      <c r="B21" s="49"/>
-      <c r="C21" s="42"/>
+      <c r="A21" s="40"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="48"/>
       <c r="D21" s="8" t="s">
         <v>14</v>
       </c>
@@ -2616,11 +2638,11 @@
       </c>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="52"/>
-      <c r="B22" s="47" t="s">
+      <c r="A22" s="40"/>
+      <c r="B22" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="44" t="s">
+      <c r="C22" s="50" t="s">
         <v>55</v>
       </c>
       <c r="D22" s="6" t="s">
@@ -2646,9 +2668,9 @@
       </c>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="52"/>
-      <c r="B23" s="48"/>
-      <c r="C23" s="45"/>
+      <c r="A23" s="40"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="51"/>
       <c r="D23" s="7" t="s">
         <v>12</v>
       </c>
@@ -2672,9 +2694,9 @@
       </c>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="52"/>
-      <c r="B24" s="48"/>
-      <c r="C24" s="45"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="51"/>
       <c r="D24" s="7" t="s">
         <v>13</v>
       </c>
@@ -2698,9 +2720,9 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A25" s="52"/>
-      <c r="B25" s="49"/>
-      <c r="C25" s="46"/>
+      <c r="A25" s="40"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="52"/>
       <c r="D25" s="8" t="s">
         <v>14</v>
       </c>
@@ -2724,11 +2746,11 @@
       </c>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="52"/>
-      <c r="B26" s="50" t="s">
+      <c r="A26" s="40"/>
+      <c r="B26" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="44" t="s">
+      <c r="C26" s="50" t="s">
         <v>96</v>
       </c>
       <c r="D26" s="9" t="s">
@@ -2754,9 +2776,9 @@
       </c>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="52"/>
-      <c r="B27" s="48"/>
-      <c r="C27" s="45"/>
+      <c r="A27" s="40"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="51"/>
       <c r="D27" s="7" t="s">
         <v>12</v>
       </c>
@@ -2780,9 +2802,9 @@
       </c>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="52"/>
-      <c r="B28" s="48"/>
-      <c r="C28" s="45"/>
+      <c r="A28" s="40"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="51"/>
       <c r="D28" s="7" t="s">
         <v>13</v>
       </c>
@@ -2806,9 +2828,9 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A29" s="52"/>
-      <c r="B29" s="49"/>
-      <c r="C29" s="46"/>
+      <c r="A29" s="40"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="52"/>
       <c r="D29" s="8" t="s">
         <v>14</v>
       </c>
@@ -2832,11 +2854,11 @@
       </c>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="52"/>
-      <c r="B30" s="50" t="s">
+      <c r="A30" s="40"/>
+      <c r="B30" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="C30" s="40" t="s">
+      <c r="C30" s="49" t="s">
         <v>120</v>
       </c>
       <c r="D30" s="9" t="s">
@@ -2862,22 +2884,35 @@
       </c>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="52"/>
-      <c r="B31" s="48"/>
-      <c r="C31" s="41"/>
+      <c r="A31" s="40"/>
+      <c r="B31" s="43"/>
+      <c r="C31" s="47"/>
       <c r="D31" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E31" s="34"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="30"/>
+      <c r="E31" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>323</v>
+      </c>
+      <c r="G31" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="H31" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="I31" s="30" t="s">
+        <v>325</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="52"/>
-      <c r="B32" s="48"/>
-      <c r="C32" s="41"/>
+      <c r="A32" s="40"/>
+      <c r="B32" s="43"/>
+      <c r="C32" s="47"/>
       <c r="D32" s="7" t="s">
         <v>13</v>
       </c>
@@ -2901,9 +2936,9 @@
       </c>
     </row>
     <row r="33" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A33" s="53"/>
-      <c r="B33" s="49"/>
-      <c r="C33" s="42"/>
+      <c r="A33" s="41"/>
+      <c r="B33" s="44"/>
+      <c r="C33" s="48"/>
       <c r="D33" s="8" t="s">
         <v>14</v>
       </c>
@@ -2927,13 +2962,13 @@
       </c>
     </row>
     <row r="34" spans="1:11">
-      <c r="A34" s="51">
+      <c r="A34" s="39">
         <v>3</v>
       </c>
-      <c r="B34" s="47" t="s">
+      <c r="B34" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C34" s="43" t="s">
+      <c r="C34" s="46" t="s">
         <v>31</v>
       </c>
       <c r="D34" s="6" t="s">
@@ -2959,9 +2994,9 @@
       </c>
     </row>
     <row r="35" spans="1:11">
-      <c r="A35" s="52"/>
-      <c r="B35" s="48"/>
-      <c r="C35" s="41"/>
+      <c r="A35" s="40"/>
+      <c r="B35" s="43"/>
+      <c r="C35" s="47"/>
       <c r="D35" s="7" t="s">
         <v>12</v>
       </c>
@@ -2985,9 +3020,9 @@
       </c>
     </row>
     <row r="36" spans="1:11">
-      <c r="A36" s="52"/>
-      <c r="B36" s="48"/>
-      <c r="C36" s="41"/>
+      <c r="A36" s="40"/>
+      <c r="B36" s="43"/>
+      <c r="C36" s="47"/>
       <c r="D36" s="7" t="s">
         <v>13</v>
       </c>
@@ -3011,9 +3046,9 @@
       </c>
     </row>
     <row r="37" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A37" s="52"/>
-      <c r="B37" s="49"/>
-      <c r="C37" s="42"/>
+      <c r="A37" s="40"/>
+      <c r="B37" s="44"/>
+      <c r="C37" s="48"/>
       <c r="D37" s="8" t="s">
         <v>14</v>
       </c>
@@ -3037,11 +3072,11 @@
       </c>
     </row>
     <row r="38" spans="1:11">
-      <c r="A38" s="52"/>
-      <c r="B38" s="47" t="s">
+      <c r="A38" s="40"/>
+      <c r="B38" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="43" t="s">
+      <c r="C38" s="46" t="s">
         <v>61</v>
       </c>
       <c r="D38" s="6" t="s">
@@ -3067,9 +3102,9 @@
       </c>
     </row>
     <row r="39" spans="1:11">
-      <c r="A39" s="52"/>
-      <c r="B39" s="48"/>
-      <c r="C39" s="41"/>
+      <c r="A39" s="40"/>
+      <c r="B39" s="43"/>
+      <c r="C39" s="47"/>
       <c r="D39" s="7" t="s">
         <v>12</v>
       </c>
@@ -3093,9 +3128,9 @@
       </c>
     </row>
     <row r="40" spans="1:11">
-      <c r="A40" s="52"/>
-      <c r="B40" s="48"/>
-      <c r="C40" s="41"/>
+      <c r="A40" s="40"/>
+      <c r="B40" s="43"/>
+      <c r="C40" s="47"/>
       <c r="D40" s="7" t="s">
         <v>13</v>
       </c>
@@ -3117,12 +3152,12 @@
       <c r="J40" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="K40" s="38"/>
+      <c r="K40" s="37"/>
     </row>
     <row r="41" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A41" s="52"/>
-      <c r="B41" s="49"/>
-      <c r="C41" s="42"/>
+      <c r="A41" s="40"/>
+      <c r="B41" s="44"/>
+      <c r="C41" s="48"/>
       <c r="D41" s="8" t="s">
         <v>14</v>
       </c>
@@ -3146,11 +3181,11 @@
       </c>
     </row>
     <row r="42" spans="1:11">
-      <c r="A42" s="52"/>
-      <c r="B42" s="50" t="s">
+      <c r="A42" s="40"/>
+      <c r="B42" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C42" s="43" t="s">
+      <c r="C42" s="46" t="s">
         <v>101</v>
       </c>
       <c r="D42" s="9" t="s">
@@ -3176,9 +3211,9 @@
       </c>
     </row>
     <row r="43" spans="1:11">
-      <c r="A43" s="52"/>
-      <c r="B43" s="48"/>
-      <c r="C43" s="41"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="43"/>
+      <c r="C43" s="47"/>
       <c r="D43" s="7" t="s">
         <v>12</v>
       </c>
@@ -3202,9 +3237,9 @@
       </c>
     </row>
     <row r="44" spans="1:11">
-      <c r="A44" s="52"/>
-      <c r="B44" s="48"/>
-      <c r="C44" s="41"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="43"/>
+      <c r="C44" s="47"/>
       <c r="D44" s="7" t="s">
         <v>13</v>
       </c>
@@ -3228,9 +3263,9 @@
       </c>
     </row>
     <row r="45" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A45" s="52"/>
-      <c r="B45" s="49"/>
-      <c r="C45" s="42"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="44"/>
+      <c r="C45" s="48"/>
       <c r="D45" s="8" t="s">
         <v>14</v>
       </c>
@@ -3254,11 +3289,11 @@
       </c>
     </row>
     <row r="46" spans="1:11">
-      <c r="A46" s="52"/>
-      <c r="B46" s="50" t="s">
+      <c r="A46" s="40"/>
+      <c r="B46" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="C46" s="40" t="s">
+      <c r="C46" s="49" t="s">
         <v>127</v>
       </c>
       <c r="D46" s="9" t="s">
@@ -3284,22 +3319,35 @@
       </c>
     </row>
     <row r="47" spans="1:11">
-      <c r="A47" s="52"/>
-      <c r="B47" s="48"/>
-      <c r="C47" s="41"/>
+      <c r="A47" s="40"/>
+      <c r="B47" s="43"/>
+      <c r="C47" s="47"/>
       <c r="D47" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E47" s="34"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="30"/>
+      <c r="E47" s="34" t="s">
+        <v>326</v>
+      </c>
+      <c r="F47" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="G47" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="H47" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="I47" s="30" t="s">
+        <v>327</v>
+      </c>
+      <c r="J47" s="4" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="48" spans="1:11">
-      <c r="A48" s="52"/>
-      <c r="B48" s="48"/>
-      <c r="C48" s="41"/>
+      <c r="A48" s="40"/>
+      <c r="B48" s="43"/>
+      <c r="C48" s="47"/>
       <c r="D48" s="7" t="s">
         <v>13</v>
       </c>
@@ -3323,9 +3371,9 @@
       </c>
     </row>
     <row r="49" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A49" s="53"/>
-      <c r="B49" s="49"/>
-      <c r="C49" s="42"/>
+      <c r="A49" s="41"/>
+      <c r="B49" s="44"/>
+      <c r="C49" s="48"/>
       <c r="D49" s="8" t="s">
         <v>14</v>
       </c>
@@ -3349,13 +3397,13 @@
       </c>
     </row>
     <row r="50" spans="1:10">
-      <c r="A50" s="51">
+      <c r="A50" s="39">
         <v>4</v>
       </c>
-      <c r="B50" s="47" t="s">
+      <c r="B50" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C50" s="43" t="s">
+      <c r="C50" s="46" t="s">
         <v>37</v>
       </c>
       <c r="D50" s="6" t="s">
@@ -3381,9 +3429,9 @@
       </c>
     </row>
     <row r="51" spans="1:10">
-      <c r="A51" s="52"/>
-      <c r="B51" s="48"/>
-      <c r="C51" s="41"/>
+      <c r="A51" s="40"/>
+      <c r="B51" s="43"/>
+      <c r="C51" s="47"/>
       <c r="D51" s="7" t="s">
         <v>12</v>
       </c>
@@ -3407,9 +3455,9 @@
       </c>
     </row>
     <row r="52" spans="1:10">
-      <c r="A52" s="52"/>
-      <c r="B52" s="48"/>
-      <c r="C52" s="41"/>
+      <c r="A52" s="40"/>
+      <c r="B52" s="43"/>
+      <c r="C52" s="47"/>
       <c r="D52" s="7" t="s">
         <v>13</v>
       </c>
@@ -3433,9 +3481,9 @@
       </c>
     </row>
     <row r="53" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A53" s="52"/>
-      <c r="B53" s="49"/>
-      <c r="C53" s="42"/>
+      <c r="A53" s="40"/>
+      <c r="B53" s="44"/>
+      <c r="C53" s="48"/>
       <c r="D53" s="8" t="s">
         <v>14</v>
       </c>
@@ -3459,11 +3507,11 @@
       </c>
     </row>
     <row r="54" spans="1:10">
-      <c r="A54" s="52"/>
-      <c r="B54" s="47" t="s">
+      <c r="A54" s="40"/>
+      <c r="B54" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C54" s="43" t="s">
+      <c r="C54" s="46" t="s">
         <v>75</v>
       </c>
       <c r="D54" s="6" t="s">
@@ -3489,9 +3537,9 @@
       </c>
     </row>
     <row r="55" spans="1:10">
-      <c r="A55" s="52"/>
-      <c r="B55" s="48"/>
-      <c r="C55" s="41"/>
+      <c r="A55" s="40"/>
+      <c r="B55" s="43"/>
+      <c r="C55" s="47"/>
       <c r="D55" s="7" t="s">
         <v>12</v>
       </c>
@@ -3515,9 +3563,9 @@
       </c>
     </row>
     <row r="56" spans="1:10">
-      <c r="A56" s="52"/>
-      <c r="B56" s="48"/>
-      <c r="C56" s="41"/>
+      <c r="A56" s="40"/>
+      <c r="B56" s="43"/>
+      <c r="C56" s="47"/>
       <c r="D56" s="7" t="s">
         <v>13</v>
       </c>
@@ -3541,9 +3589,9 @@
       </c>
     </row>
     <row r="57" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A57" s="52"/>
-      <c r="B57" s="49"/>
-      <c r="C57" s="42"/>
+      <c r="A57" s="40"/>
+      <c r="B57" s="44"/>
+      <c r="C57" s="48"/>
       <c r="D57" s="8" t="s">
         <v>14</v>
       </c>
@@ -3567,11 +3615,11 @@
       </c>
     </row>
     <row r="58" spans="1:10">
-      <c r="A58" s="52"/>
-      <c r="B58" s="50" t="s">
+      <c r="A58" s="40"/>
+      <c r="B58" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C58" s="43" t="s">
+      <c r="C58" s="46" t="s">
         <v>108</v>
       </c>
       <c r="D58" s="9" t="s">
@@ -3597,9 +3645,9 @@
       </c>
     </row>
     <row r="59" spans="1:10">
-      <c r="A59" s="52"/>
-      <c r="B59" s="48"/>
-      <c r="C59" s="41"/>
+      <c r="A59" s="40"/>
+      <c r="B59" s="43"/>
+      <c r="C59" s="47"/>
       <c r="D59" s="7" t="s">
         <v>12</v>
       </c>
@@ -3623,9 +3671,9 @@
       </c>
     </row>
     <row r="60" spans="1:10">
-      <c r="A60" s="52"/>
-      <c r="B60" s="48"/>
-      <c r="C60" s="41"/>
+      <c r="A60" s="40"/>
+      <c r="B60" s="43"/>
+      <c r="C60" s="47"/>
       <c r="D60" s="7" t="s">
         <v>13</v>
       </c>
@@ -3649,9 +3697,9 @@
       </c>
     </row>
     <row r="61" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A61" s="52"/>
-      <c r="B61" s="49"/>
-      <c r="C61" s="42"/>
+      <c r="A61" s="40"/>
+      <c r="B61" s="44"/>
+      <c r="C61" s="48"/>
       <c r="D61" s="8" t="s">
         <v>14</v>
       </c>
@@ -3675,11 +3723,11 @@
       </c>
     </row>
     <row r="62" spans="1:10">
-      <c r="A62" s="52"/>
-      <c r="B62" s="50" t="s">
+      <c r="A62" s="40"/>
+      <c r="B62" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="C62" s="40" t="s">
+      <c r="C62" s="49" t="s">
         <v>134</v>
       </c>
       <c r="D62" s="9" t="s">
@@ -3705,22 +3753,35 @@
       </c>
     </row>
     <row r="63" spans="1:10">
-      <c r="A63" s="52"/>
-      <c r="B63" s="48"/>
-      <c r="C63" s="41"/>
+      <c r="A63" s="40"/>
+      <c r="B63" s="43"/>
+      <c r="C63" s="47"/>
       <c r="D63" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E63" s="34"/>
-      <c r="F63" s="14"/>
-      <c r="G63" s="14"/>
-      <c r="H63" s="14"/>
-      <c r="I63" s="30"/>
+      <c r="E63" s="34" t="s">
+        <v>328</v>
+      </c>
+      <c r="F63" s="14" t="s">
+        <v>301</v>
+      </c>
+      <c r="G63" s="14" t="s">
+        <v>329</v>
+      </c>
+      <c r="H63" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="I63" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="J63" s="4" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="64" spans="1:10">
-      <c r="A64" s="52"/>
-      <c r="B64" s="48"/>
-      <c r="C64" s="41"/>
+      <c r="A64" s="40"/>
+      <c r="B64" s="43"/>
+      <c r="C64" s="47"/>
       <c r="D64" s="7" t="s">
         <v>13</v>
       </c>
@@ -3744,9 +3805,9 @@
       </c>
     </row>
     <row r="65" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A65" s="53"/>
-      <c r="B65" s="49"/>
-      <c r="C65" s="42"/>
+      <c r="A65" s="41"/>
+      <c r="B65" s="44"/>
+      <c r="C65" s="48"/>
       <c r="D65" s="8" t="s">
         <v>14</v>
       </c>
@@ -3770,13 +3831,13 @@
       </c>
     </row>
     <row r="66" spans="1:10">
-      <c r="A66" s="51">
+      <c r="A66" s="39">
         <v>5</v>
       </c>
-      <c r="B66" s="47" t="s">
+      <c r="B66" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C66" s="43" t="s">
+      <c r="C66" s="46" t="s">
         <v>43</v>
       </c>
       <c r="D66" s="6" t="s">
@@ -3802,9 +3863,9 @@
       </c>
     </row>
     <row r="67" spans="1:10">
-      <c r="A67" s="52"/>
-      <c r="B67" s="48"/>
-      <c r="C67" s="41"/>
+      <c r="A67" s="40"/>
+      <c r="B67" s="43"/>
+      <c r="C67" s="47"/>
       <c r="D67" s="7" t="s">
         <v>12</v>
       </c>
@@ -3828,9 +3889,9 @@
       </c>
     </row>
     <row r="68" spans="1:10">
-      <c r="A68" s="52"/>
-      <c r="B68" s="48"/>
-      <c r="C68" s="41"/>
+      <c r="A68" s="40"/>
+      <c r="B68" s="43"/>
+      <c r="C68" s="47"/>
       <c r="D68" s="7" t="s">
         <v>13</v>
       </c>
@@ -3854,9 +3915,9 @@
       </c>
     </row>
     <row r="69" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A69" s="52"/>
-      <c r="B69" s="49"/>
-      <c r="C69" s="42"/>
+      <c r="A69" s="40"/>
+      <c r="B69" s="44"/>
+      <c r="C69" s="48"/>
       <c r="D69" s="8" t="s">
         <v>14</v>
       </c>
@@ -3880,11 +3941,11 @@
       </c>
     </row>
     <row r="70" spans="1:10">
-      <c r="A70" s="52"/>
-      <c r="B70" s="47" t="s">
+      <c r="A70" s="40"/>
+      <c r="B70" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C70" s="43" t="s">
+      <c r="C70" s="46" t="s">
         <v>82</v>
       </c>
       <c r="D70" s="6" t="s">
@@ -3910,9 +3971,9 @@
       </c>
     </row>
     <row r="71" spans="1:10">
-      <c r="A71" s="52"/>
-      <c r="B71" s="48"/>
-      <c r="C71" s="41"/>
+      <c r="A71" s="40"/>
+      <c r="B71" s="43"/>
+      <c r="C71" s="47"/>
       <c r="D71" s="7" t="s">
         <v>12</v>
       </c>
@@ -3936,9 +3997,9 @@
       </c>
     </row>
     <row r="72" spans="1:10">
-      <c r="A72" s="52"/>
-      <c r="B72" s="48"/>
-      <c r="C72" s="41"/>
+      <c r="A72" s="40"/>
+      <c r="B72" s="43"/>
+      <c r="C72" s="47"/>
       <c r="D72" s="7" t="s">
         <v>13</v>
       </c>
@@ -3962,9 +4023,9 @@
       </c>
     </row>
     <row r="73" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A73" s="52"/>
-      <c r="B73" s="49"/>
-      <c r="C73" s="42"/>
+      <c r="A73" s="40"/>
+      <c r="B73" s="44"/>
+      <c r="C73" s="48"/>
       <c r="D73" s="8" t="s">
         <v>14</v>
       </c>
@@ -3988,11 +4049,11 @@
       </c>
     </row>
     <row r="74" spans="1:10">
-      <c r="A74" s="52"/>
-      <c r="B74" s="50" t="s">
+      <c r="A74" s="40"/>
+      <c r="B74" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C74" s="43" t="s">
+      <c r="C74" s="46" t="s">
         <v>115</v>
       </c>
       <c r="D74" s="9" t="s">
@@ -4018,9 +4079,9 @@
       </c>
     </row>
     <row r="75" spans="1:10">
-      <c r="A75" s="52"/>
-      <c r="B75" s="48"/>
-      <c r="C75" s="41"/>
+      <c r="A75" s="40"/>
+      <c r="B75" s="43"/>
+      <c r="C75" s="47"/>
       <c r="D75" s="7" t="s">
         <v>12</v>
       </c>
@@ -4044,9 +4105,9 @@
       </c>
     </row>
     <row r="76" spans="1:10">
-      <c r="A76" s="52"/>
-      <c r="B76" s="48"/>
-      <c r="C76" s="41"/>
+      <c r="A76" s="40"/>
+      <c r="B76" s="43"/>
+      <c r="C76" s="47"/>
       <c r="D76" s="7" t="s">
         <v>13</v>
       </c>
@@ -4070,9 +4131,9 @@
       </c>
     </row>
     <row r="77" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A77" s="52"/>
-      <c r="B77" s="49"/>
-      <c r="C77" s="42"/>
+      <c r="A77" s="40"/>
+      <c r="B77" s="44"/>
+      <c r="C77" s="48"/>
       <c r="D77" s="8" t="s">
         <v>14</v>
       </c>
@@ -4096,11 +4157,11 @@
       </c>
     </row>
     <row r="78" spans="1:10">
-      <c r="A78" s="52"/>
-      <c r="B78" s="50" t="s">
+      <c r="A78" s="40"/>
+      <c r="B78" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="C78" s="40" t="s">
+      <c r="C78" s="49" t="s">
         <v>141</v>
       </c>
       <c r="D78" s="9" t="s">
@@ -4126,22 +4187,35 @@
       </c>
     </row>
     <row r="79" spans="1:10">
-      <c r="A79" s="52"/>
-      <c r="B79" s="48"/>
-      <c r="C79" s="41"/>
+      <c r="A79" s="40"/>
+      <c r="B79" s="43"/>
+      <c r="C79" s="47"/>
       <c r="D79" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E79" s="34"/>
-      <c r="F79" s="14"/>
-      <c r="G79" s="14"/>
-      <c r="H79" s="14"/>
-      <c r="I79" s="30"/>
+      <c r="E79" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="F79" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="G79" s="14" t="s">
+        <v>331</v>
+      </c>
+      <c r="H79" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="I79" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="J79" s="4" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="80" spans="1:10">
-      <c r="A80" s="52"/>
-      <c r="B80" s="48"/>
-      <c r="C80" s="41"/>
+      <c r="A80" s="40"/>
+      <c r="B80" s="43"/>
+      <c r="C80" s="47"/>
       <c r="D80" s="7" t="s">
         <v>13</v>
       </c>
@@ -4165,9 +4239,9 @@
       </c>
     </row>
     <row r="81" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A81" s="53"/>
-      <c r="B81" s="49"/>
-      <c r="C81" s="42"/>
+      <c r="A81" s="41"/>
+      <c r="B81" s="44"/>
+      <c r="C81" s="48"/>
       <c r="D81" s="8" t="s">
         <v>14</v>
       </c>
@@ -4912,51 +4986,51 @@
     </row>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="C78:C81"/>
+    <mergeCell ref="C54:C57"/>
+    <mergeCell ref="C58:C61"/>
+    <mergeCell ref="C70:C73"/>
+    <mergeCell ref="C74:C77"/>
+    <mergeCell ref="C50:C53"/>
+    <mergeCell ref="C38:C41"/>
+    <mergeCell ref="C42:C45"/>
+    <mergeCell ref="C62:C65"/>
+    <mergeCell ref="C66:C69"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="C46:C49"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="A2:A17"/>
+    <mergeCell ref="A34:A49"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="A18:A33"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="A66:A81"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="B70:B73"/>
+    <mergeCell ref="B74:B77"/>
+    <mergeCell ref="B78:B81"/>
     <mergeCell ref="A50:A65"/>
     <mergeCell ref="B50:B53"/>
     <mergeCell ref="B54:B57"/>
     <mergeCell ref="B58:B61"/>
     <mergeCell ref="B62:B65"/>
-    <mergeCell ref="A66:A81"/>
-    <mergeCell ref="B66:B69"/>
-    <mergeCell ref="B70:B73"/>
-    <mergeCell ref="B74:B77"/>
-    <mergeCell ref="B78:B81"/>
-    <mergeCell ref="A18:A33"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="A34:A49"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A2:A17"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="C46:C49"/>
-    <mergeCell ref="C50:C53"/>
-    <mergeCell ref="C38:C41"/>
-    <mergeCell ref="C42:C45"/>
-    <mergeCell ref="C62:C65"/>
-    <mergeCell ref="C66:C69"/>
-    <mergeCell ref="C78:C81"/>
-    <mergeCell ref="C54:C57"/>
-    <mergeCell ref="C58:C61"/>
-    <mergeCell ref="C70:C73"/>
-    <mergeCell ref="C74:C77"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>